<commit_message>
added dtu materials to sampling
</commit_message>
<xml_diff>
--- a/delphin_6_automation/sampling/input_files/Brick.xlsx
+++ b/delphin_6_automation/sampling/input_files/Brick.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Material ID</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>ZiegelSchlagmannWDZZiegelhuelle</t>
+  </si>
+  <si>
+    <t>DTUBrick</t>
   </si>
 </sst>
 </file>
@@ -542,19 +545,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>33</v>
       </c>
@@ -570,7 +573,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>34</v>
       </c>
@@ -578,7 +581,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>96</v>
       </c>
@@ -586,7 +589,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>97</v>
       </c>
@@ -594,7 +597,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>98</v>
       </c>
@@ -602,7 +605,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>152</v>
       </c>
@@ -610,7 +613,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>153</v>
       </c>
@@ -618,7 +621,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>264</v>
       </c>
@@ -626,7 +629,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>286</v>
       </c>
@@ -634,7 +637,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>490</v>
       </c>
@@ -642,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>491</v>
       </c>
@@ -650,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>492</v>
       </c>
@@ -658,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>493</v>
       </c>
@@ -666,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>494</v>
       </c>
@@ -674,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>495</v>
       </c>
@@ -682,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>496</v>
       </c>
@@ -690,7 +693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>497</v>
       </c>
@@ -698,7 +701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>498</v>
       </c>
@@ -706,7 +709,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>499</v>
       </c>
@@ -714,7 +717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>500</v>
       </c>
@@ -722,7 +725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>501</v>
       </c>
@@ -730,7 +733,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>502</v>
       </c>
@@ -738,7 +741,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>503</v>
       </c>
@@ -746,7 +749,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>505</v>
       </c>
@@ -754,7 +757,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>506</v>
       </c>
@@ -762,7 +765,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>507</v>
       </c>
@@ -770,7 +773,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>508</v>
       </c>
@@ -778,7 +781,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>509</v>
       </c>
@@ -786,7 +789,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>510</v>
       </c>
@@ -794,7 +797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>511</v>
       </c>
@@ -802,7 +805,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>512</v>
       </c>
@@ -810,7 +813,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>513</v>
       </c>
@@ -818,7 +821,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>528</v>
       </c>
@@ -826,7 +829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>529</v>
       </c>
@@ -834,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>530</v>
       </c>
@@ -842,7 +845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>531</v>
       </c>
@@ -850,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>532</v>
       </c>
@@ -858,7 +861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>533</v>
       </c>
@@ -866,7 +869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>534</v>
       </c>
@@ -874,7 +877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>535</v>
       </c>
@@ -882,7 +885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>536</v>
       </c>
@@ -890,7 +893,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>537</v>
       </c>
@@ -898,7 +901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>538</v>
       </c>
@@ -906,7 +909,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>539</v>
       </c>
@@ -914,7 +917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>540</v>
       </c>
@@ -922,7 +925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>541</v>
       </c>
@@ -930,7 +933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>542</v>
       </c>
@@ -938,7 +941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>543</v>
       </c>
@@ -946,7 +949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>544</v>
       </c>
@@ -954,7 +957,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>545</v>
       </c>
@@ -962,7 +965,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>546</v>
       </c>
@@ -970,7 +973,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>547</v>
       </c>
@@ -978,7 +981,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>548</v>
       </c>
@@ -986,7 +989,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>549</v>
       </c>
@@ -994,7 +997,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>550</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>551</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>552</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>557</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>685</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>686</v>
       </c>
@@ -1042,12 +1045,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>791</v>
       </c>
       <c r="B62" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>901</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>